<commit_message>
national csv format and config file updates
match scalar names
</commit_message>
<xml_diff>
--- a/inst/extdata/fredi/national/FrEDI_config.xlsx
+++ b/inst/extdata/fredi/national/FrEDI_config.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr filterPrivacy="1" updateLinks="never" codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D91DE60B-0F56-40B0-B073-ECBDC5B00A65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0931E3-6248-41F5-B806-AFA6CD657CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="764" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2380,24 +2380,9 @@
     <t>elecTD_growthFactor_nat</t>
   </si>
   <si>
-    <t>forestryLoss_growthFactor_SSP2_nat</t>
-  </si>
-  <si>
-    <t>forestryLoss_growthFactor_SSP5_nat</t>
-  </si>
-  <si>
     <t>rail_growth_factor_nat</t>
   </si>
   <si>
-    <t>road_miles_and_pop_NoAdapt_nat</t>
-  </si>
-  <si>
-    <t>road_miles_and_pop_Proactive_nat</t>
-  </si>
-  <si>
-    <t>road_miles_and_pop_Reactive_nat</t>
-  </si>
-  <si>
     <t>SouthwestDust_pop_nat</t>
   </si>
   <si>
@@ -2570,6 +2555,21 @@
   </si>
   <si>
     <t>65-99 Population Proportion Adjustment Factor BenMAP combined with SW state population subset</t>
+  </si>
+  <si>
+    <t>forestryLoss_growthFactor_nat_SSP2</t>
+  </si>
+  <si>
+    <t>forestryLoss_growthFactor_nat_SSP5</t>
+  </si>
+  <si>
+    <t>road_miles_and_pop_nat_NoAdapt</t>
+  </si>
+  <si>
+    <t>road_miles_and_pop_nat_Proactive</t>
+  </si>
+  <si>
+    <t>road_miles_and_pop_nat_Reactive</t>
   </si>
 </sst>
 </file>
@@ -9967,9 +9967,9 @@
   </sheetPr>
   <dimension ref="A1:U407"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A227" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H221" sqref="H221"/>
+      <selection pane="topRight" activeCell="E236" sqref="E236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14842,13 +14842,13 @@
         <v>84</v>
       </c>
       <c r="I154" s="28" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="J154" s="32" t="s">
         <v>683</v>
       </c>
       <c r="K154" s="28" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="L154" s="28" t="s">
         <v>88</v>
@@ -14891,13 +14891,13 @@
         <v>84</v>
       </c>
       <c r="I155" s="28" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="J155" s="32" t="s">
         <v>684</v>
       </c>
       <c r="K155" s="28" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="L155" s="28" t="s">
         <v>89</v>
@@ -14940,13 +14940,13 @@
         <v>84</v>
       </c>
       <c r="I156" s="32" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="J156" s="32" t="s">
         <v>685</v>
       </c>
       <c r="K156" s="32" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="L156" s="28" t="s">
         <v>89</v>
@@ -14989,13 +14989,13 @@
         <v>84</v>
       </c>
       <c r="I157" s="32" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="J157" s="32" t="s">
         <v>686</v>
       </c>
       <c r="K157" s="28" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="L157" s="28" t="s">
         <v>88</v>
@@ -15038,13 +15038,13 @@
         <v>84</v>
       </c>
       <c r="I158" s="28" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="J158" s="32" t="s">
         <v>687</v>
       </c>
       <c r="K158" s="28" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="L158" s="28" t="s">
         <v>89</v>
@@ -15084,7 +15084,7 @@
         <v>532</v>
       </c>
       <c r="H159" s="28" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="I159" s="28" t="s">
         <v>88</v>
@@ -15387,7 +15387,7 @@
         <v>88</v>
       </c>
       <c r="K165" s="28" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="L165" s="28" t="s">
         <v>88</v>
@@ -15436,7 +15436,7 @@
         <v>88</v>
       </c>
       <c r="K166" s="28" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="L166" s="28" t="s">
         <v>88</v>
@@ -15675,7 +15675,7 @@
         <v>84</v>
       </c>
       <c r="I171" s="28" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="J171" s="28" t="s">
         <v>88</v>
@@ -15724,7 +15724,7 @@
         <v>84</v>
       </c>
       <c r="I172" s="28" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="J172" s="28" t="s">
         <v>88</v>
@@ -15776,7 +15776,7 @@
         <v>88</v>
       </c>
       <c r="J173" s="28" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="K173" s="28" t="s">
         <v>89</v>
@@ -15917,7 +15917,7 @@
         <v>533</v>
       </c>
       <c r="H176" s="28" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="I176" s="28" t="s">
         <v>88</v>
@@ -15926,7 +15926,7 @@
         <v>88</v>
       </c>
       <c r="K176" s="28" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="L176" s="28" t="s">
         <v>89</v>
@@ -15969,7 +15969,7 @@
         <v>84</v>
       </c>
       <c r="I177" s="28" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="J177" s="28" t="s">
         <v>88</v>
@@ -16018,7 +16018,7 @@
         <v>84</v>
       </c>
       <c r="I178" s="28" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="J178" s="28" t="s">
         <v>88</v>
@@ -16067,13 +16067,13 @@
         <v>84</v>
       </c>
       <c r="I179" s="32" t="s">
-        <v>734</v>
+        <v>729</v>
       </c>
       <c r="J179" s="28" t="s">
         <v>88</v>
       </c>
       <c r="K179" s="28" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="L179" s="28" t="s">
         <v>88</v>
@@ -16410,13 +16410,13 @@
         <v>84</v>
       </c>
       <c r="I186" s="28" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="J186" s="28" t="s">
         <v>88</v>
       </c>
       <c r="K186" s="28" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="L186" s="28" t="s">
         <v>88</v>
@@ -16459,13 +16459,13 @@
         <v>84</v>
       </c>
       <c r="I187" s="28" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="J187" s="28" t="s">
         <v>88</v>
       </c>
       <c r="K187" s="28" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="L187" s="28" t="s">
         <v>88</v>
@@ -16508,13 +16508,13 @@
         <v>84</v>
       </c>
       <c r="I188" s="28" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="J188" s="28" t="s">
         <v>88</v>
       </c>
       <c r="K188" s="28" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="L188" s="28" t="s">
         <v>88</v>
@@ -16557,7 +16557,7 @@
         <v>84</v>
       </c>
       <c r="I189" s="28" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="J189" s="28" t="s">
         <v>88</v>
@@ -16606,7 +16606,7 @@
         <v>84</v>
       </c>
       <c r="I190" s="28" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="J190" s="28" t="s">
         <v>88</v>
@@ -16655,10 +16655,10 @@
         <v>84</v>
       </c>
       <c r="I191" s="28" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="J191" s="28" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="K191" s="28" t="s">
         <v>119</v>
@@ -16701,13 +16701,13 @@
         <v>52</v>
       </c>
       <c r="H192" s="28" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="I192" s="25" t="s">
         <v>88</v>
       </c>
       <c r="J192" s="25" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="K192" s="28" t="s">
         <v>88</v>
@@ -16750,13 +16750,13 @@
         <v>126</v>
       </c>
       <c r="H193" s="28" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="I193" s="25" t="s">
         <v>88</v>
       </c>
       <c r="J193" s="25" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="K193" s="28" t="s">
         <v>88</v>
@@ -16802,13 +16802,13 @@
         <v>84</v>
       </c>
       <c r="I194" s="32" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="J194" s="28" t="s">
         <v>88</v>
       </c>
       <c r="K194" s="28" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="L194" s="28" t="s">
         <v>88</v>
@@ -16851,13 +16851,13 @@
         <v>84</v>
       </c>
       <c r="I195" s="32" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="J195" s="28" t="s">
         <v>88</v>
       </c>
       <c r="K195" s="28" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="L195" s="28" t="s">
         <v>88</v>
@@ -16900,7 +16900,7 @@
         <v>84</v>
       </c>
       <c r="I196" s="32" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="J196" s="28" t="s">
         <v>88</v>
@@ -16949,13 +16949,13 @@
         <v>84</v>
       </c>
       <c r="I197" s="32" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="J197" s="28" t="s">
         <v>88</v>
       </c>
       <c r="K197" s="28" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="L197" s="28" t="s">
         <v>88</v>
@@ -16998,13 +16998,13 @@
         <v>84</v>
       </c>
       <c r="I198" s="28" t="s">
-        <v>735</v>
+        <v>730</v>
       </c>
       <c r="J198" s="28" t="s">
         <v>88</v>
       </c>
       <c r="K198" s="28" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="L198" s="28" t="s">
         <v>88</v>
@@ -17047,13 +17047,13 @@
         <v>84</v>
       </c>
       <c r="I199" s="32" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="J199" s="32" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="K199" s="32" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="L199" s="28" t="s">
         <v>89</v>
@@ -17146,13 +17146,13 @@
         <v>84</v>
       </c>
       <c r="I201" s="28" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="J201" s="28" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="K201" s="28" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="L201" s="28" t="s">
         <v>89</v>
@@ -17195,13 +17195,13 @@
         <v>84</v>
       </c>
       <c r="I202" s="28" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="J202" s="28" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="K202" s="28" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="L202" s="28" t="s">
         <v>88</v>
@@ -17244,10 +17244,10 @@
         <v>84</v>
       </c>
       <c r="I203" s="28" t="s">
-        <v>736</v>
+        <v>731</v>
       </c>
       <c r="J203" s="28" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="K203" s="28" t="s">
         <v>119</v>
@@ -17348,7 +17348,7 @@
         <v>88</v>
       </c>
       <c r="K205" s="28" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="L205" s="28" t="s">
         <v>89</v>
@@ -17593,7 +17593,7 @@
         <v>88</v>
       </c>
       <c r="K210" s="28" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="L210" s="28" t="s">
         <v>88</v>
@@ -17636,13 +17636,13 @@
         <v>84</v>
       </c>
       <c r="I211" s="28" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="J211" s="32" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="K211" s="28" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="L211" s="28" t="s">
         <v>89</v>
@@ -17734,7 +17734,7 @@
         <v>84</v>
       </c>
       <c r="I213" s="32" t="s">
-        <v>737</v>
+        <v>732</v>
       </c>
       <c r="J213" s="28" t="s">
         <v>88</v>
@@ -17783,7 +17783,7 @@
         <v>84</v>
       </c>
       <c r="I214" s="32" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="J214" s="28" t="s">
         <v>88</v>
@@ -17832,7 +17832,7 @@
         <v>84</v>
       </c>
       <c r="I215" s="32" t="s">
-        <v>738</v>
+        <v>733</v>
       </c>
       <c r="J215" s="28" t="s">
         <v>88</v>
@@ -18149,7 +18149,7 @@
         <v>8</v>
       </c>
       <c r="C228" s="32" t="s">
-        <v>690</v>
+        <v>749</v>
       </c>
       <c r="D228" s="26" t="s">
         <v>627</v>
@@ -18180,7 +18180,7 @@
         <v>9</v>
       </c>
       <c r="C229" s="32" t="s">
-        <v>691</v>
+        <v>750</v>
       </c>
       <c r="D229" s="26" t="s">
         <v>628</v>
@@ -18244,7 +18244,7 @@
         <v>11</v>
       </c>
       <c r="C231" s="32" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="D231" s="26" t="s">
         <v>128</v>
@@ -18275,7 +18275,7 @@
         <v>12</v>
       </c>
       <c r="C232" s="32" t="s">
-        <v>693</v>
+        <v>751</v>
       </c>
       <c r="D232" s="26" t="s">
         <v>538</v>
@@ -18308,7 +18308,7 @@
         <v>13</v>
       </c>
       <c r="C233" s="32" t="s">
-        <v>694</v>
+        <v>752</v>
       </c>
       <c r="D233" s="26" t="s">
         <v>539</v>
@@ -18341,7 +18341,7 @@
         <v>14</v>
       </c>
       <c r="C234" s="32" t="s">
-        <v>695</v>
+        <v>753</v>
       </c>
       <c r="D234" s="26" t="s">
         <v>540</v>
@@ -18374,7 +18374,7 @@
         <v>15</v>
       </c>
       <c r="C235" s="32" t="s">
-        <v>696</v>
+        <v>691</v>
       </c>
       <c r="D235" s="26" t="s">
         <v>668</v>
@@ -18407,7 +18407,7 @@
         <v>16</v>
       </c>
       <c r="C236" s="32" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="D236" s="26" t="s">
         <v>663</v>
@@ -18440,7 +18440,7 @@
         <v>17</v>
       </c>
       <c r="C237" s="32" t="s">
-        <v>698</v>
+        <v>693</v>
       </c>
       <c r="D237" s="26" t="s">
         <v>664</v>
@@ -18471,7 +18471,7 @@
         <v>18</v>
       </c>
       <c r="C238" s="28" t="s">
-        <v>699</v>
+        <v>694</v>
       </c>
       <c r="D238" s="26" t="s">
         <v>665</v>
@@ -18502,7 +18502,7 @@
         <v>19</v>
       </c>
       <c r="C239" s="32" t="s">
-        <v>700</v>
+        <v>695</v>
       </c>
       <c r="D239" s="26" t="s">
         <v>666</v>
@@ -18533,7 +18533,7 @@
         <v>20</v>
       </c>
       <c r="C240" s="32" t="s">
-        <v>701</v>
+        <v>696</v>
       </c>
       <c r="D240" s="26" t="s">
         <v>240</v>
@@ -18564,7 +18564,7 @@
         <v>21</v>
       </c>
       <c r="C241" s="32" t="s">
-        <v>702</v>
+        <v>697</v>
       </c>
       <c r="D241" s="26" t="s">
         <v>615</v>
@@ -18595,7 +18595,7 @@
         <v>22</v>
       </c>
       <c r="C242" s="32" t="s">
-        <v>703</v>
+        <v>698</v>
       </c>
       <c r="D242" s="26" t="s">
         <v>630</v>
@@ -18626,7 +18626,7 @@
         <v>23</v>
       </c>
       <c r="C243" s="26" t="s">
-        <v>704</v>
+        <v>699</v>
       </c>
       <c r="D243" s="26" t="s">
         <v>102</v>
@@ -18657,7 +18657,7 @@
         <v>24</v>
       </c>
       <c r="C244" s="32" t="s">
-        <v>705</v>
+        <v>700</v>
       </c>
       <c r="D244" s="26" t="s">
         <v>122</v>
@@ -18688,7 +18688,7 @@
         <v>25</v>
       </c>
       <c r="C245" s="32" t="s">
-        <v>706</v>
+        <v>701</v>
       </c>
       <c r="D245" s="26" t="s">
         <v>120</v>
@@ -18716,7 +18716,7 @@
         <v>26</v>
       </c>
       <c r="C246" s="32" t="s">
-        <v>707</v>
+        <v>702</v>
       </c>
       <c r="D246" s="26" t="s">
         <v>121</v>
@@ -18744,7 +18744,7 @@
         <v>27</v>
       </c>
       <c r="C247" s="32" t="s">
-        <v>708</v>
+        <v>703</v>
       </c>
       <c r="D247" s="26" t="s">
         <v>596</v>
@@ -18802,7 +18802,7 @@
         <v>29</v>
       </c>
       <c r="C249" s="32" t="s">
-        <v>709</v>
+        <v>704</v>
       </c>
       <c r="D249" s="26" t="s">
         <v>342</v>
@@ -18828,7 +18828,7 @@
         <v>30</v>
       </c>
       <c r="C250" s="32" t="s">
-        <v>710</v>
+        <v>705</v>
       </c>
       <c r="D250" s="26" t="s">
         <v>616</v>
@@ -18856,7 +18856,7 @@
         <v>31</v>
       </c>
       <c r="C251" s="28" t="s">
-        <v>711</v>
+        <v>706</v>
       </c>
       <c r="D251" s="26" t="s">
         <v>672</v>
@@ -18884,7 +18884,7 @@
         <v>32</v>
       </c>
       <c r="C252" s="32" t="s">
-        <v>712</v>
+        <v>707</v>
       </c>
       <c r="D252" s="26" t="s">
         <v>241</v>
@@ -18912,7 +18912,7 @@
         <v>33</v>
       </c>
       <c r="C253" s="32" t="s">
-        <v>713</v>
+        <v>708</v>
       </c>
       <c r="D253" s="26" t="s">
         <v>343</v>
@@ -18938,7 +18938,7 @@
         <v>34</v>
       </c>
       <c r="C254" s="26" t="s">
-        <v>714</v>
+        <v>709</v>
       </c>
       <c r="D254" s="26" t="s">
         <v>16</v>
@@ -18966,7 +18966,7 @@
         <v>35</v>
       </c>
       <c r="C255" s="32" t="s">
-        <v>715</v>
+        <v>710</v>
       </c>
       <c r="D255" s="26" t="s">
         <v>617</v>
@@ -18994,7 +18994,7 @@
         <v>36</v>
       </c>
       <c r="C256" s="28" t="s">
-        <v>716</v>
+        <v>711</v>
       </c>
       <c r="D256" s="26" t="s">
         <v>667</v>
@@ -19022,7 +19022,7 @@
         <v>37</v>
       </c>
       <c r="C257" s="32" t="s">
-        <v>717</v>
+        <v>712</v>
       </c>
       <c r="D257" s="26" t="s">
         <v>105</v>
@@ -19080,7 +19080,7 @@
         <v>39</v>
       </c>
       <c r="C259" s="32" t="s">
-        <v>718</v>
+        <v>713</v>
       </c>
       <c r="D259" s="26" t="s">
         <v>238</v>
@@ -19108,7 +19108,7 @@
         <v>40</v>
       </c>
       <c r="C260" s="32" t="s">
-        <v>719</v>
+        <v>714</v>
       </c>
       <c r="D260" s="26" t="s">
         <v>237</v>
@@ -19136,7 +19136,7 @@
         <v>41</v>
       </c>
       <c r="C261" s="32" t="s">
-        <v>720</v>
+        <v>715</v>
       </c>
       <c r="D261" s="26" t="s">
         <v>239</v>
@@ -19164,7 +19164,7 @@
         <v>42</v>
       </c>
       <c r="C262" s="32" t="s">
-        <v>721</v>
+        <v>716</v>
       </c>
       <c r="D262" s="26" t="s">
         <v>255</v>
@@ -19192,7 +19192,7 @@
         <v>43</v>
       </c>
       <c r="C263" s="32" t="s">
-        <v>722</v>
+        <v>717</v>
       </c>
       <c r="D263" s="26" t="s">
         <v>95</v>
@@ -19250,7 +19250,7 @@
         <v>45</v>
       </c>
       <c r="C265" s="32" t="s">
-        <v>723</v>
+        <v>718</v>
       </c>
       <c r="D265" s="26" t="s">
         <v>52</v>
@@ -19278,7 +19278,7 @@
         <v>46</v>
       </c>
       <c r="C266" s="32" t="s">
-        <v>724</v>
+        <v>719</v>
       </c>
       <c r="D266" s="26" t="s">
         <v>48</v>
@@ -19306,7 +19306,7 @@
         <v>47</v>
       </c>
       <c r="C267" s="32" t="s">
-        <v>725</v>
+        <v>720</v>
       </c>
       <c r="D267" s="26" t="s">
         <v>126</v>
@@ -19334,10 +19334,10 @@
         <v>48</v>
       </c>
       <c r="C268" s="32" t="s">
-        <v>732</v>
+        <v>727</v>
       </c>
       <c r="D268" s="26" t="s">
-        <v>733</v>
+        <v>728</v>
       </c>
       <c r="E268" s="80" t="s">
         <v>157</v>
@@ -19362,10 +19362,10 @@
         <v>49</v>
       </c>
       <c r="C269" s="32" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
       <c r="D269" s="26" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
       <c r="E269" s="80" t="s">
         <v>157</v>
@@ -19390,7 +19390,7 @@
         <v>50</v>
       </c>
       <c r="C270" s="32" t="s">
-        <v>726</v>
+        <v>721</v>
       </c>
       <c r="D270" s="26" t="s">
         <v>670</v>
@@ -19418,7 +19418,7 @@
         <v>51</v>
       </c>
       <c r="C271" s="32" t="s">
-        <v>727</v>
+        <v>722</v>
       </c>
       <c r="D271" s="26" t="s">
         <v>671</v>
@@ -19446,10 +19446,10 @@
         <v>52</v>
       </c>
       <c r="C272" s="32" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
       <c r="D272" s="26" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="E272" s="80" t="s">
         <v>157</v>
@@ -19474,10 +19474,10 @@
         <v>53</v>
       </c>
       <c r="C273" s="32" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
       <c r="D273" s="26" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
       <c r="E273" s="80" t="s">
         <v>157</v>
@@ -19502,10 +19502,10 @@
         <v>54</v>
       </c>
       <c r="C274" s="32" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="D274" s="26" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="E274" s="80" t="s">
         <v>157</v>
@@ -19530,7 +19530,7 @@
         <v>55</v>
       </c>
       <c r="C275" s="32" t="s">
-        <v>728</v>
+        <v>723</v>
       </c>
       <c r="D275" s="26" t="s">
         <v>641</v>
@@ -19558,10 +19558,10 @@
         <v>56</v>
       </c>
       <c r="C276" s="26" t="s">
+        <v>729</v>
+      </c>
+      <c r="D276" s="26" t="s">
         <v>734</v>
-      </c>
-      <c r="D276" s="26" t="s">
-        <v>739</v>
       </c>
       <c r="E276" s="80" t="s">
         <v>157</v>
@@ -19586,10 +19586,10 @@
         <v>57</v>
       </c>
       <c r="C277" s="26" t="s">
+        <v>730</v>
+      </c>
+      <c r="D277" s="26" t="s">
         <v>735</v>
-      </c>
-      <c r="D277" s="26" t="s">
-        <v>740</v>
       </c>
       <c r="E277" s="80" t="s">
         <v>157</v>
@@ -19614,10 +19614,10 @@
         <v>58</v>
       </c>
       <c r="C278" s="26" t="s">
+        <v>731</v>
+      </c>
+      <c r="D278" s="26" t="s">
         <v>736</v>
-      </c>
-      <c r="D278" s="26" t="s">
-        <v>741</v>
       </c>
       <c r="E278" s="80" t="s">
         <v>157</v>
@@ -19642,10 +19642,10 @@
         <v>59</v>
       </c>
       <c r="C279" s="32" t="s">
+        <v>732</v>
+      </c>
+      <c r="D279" s="26" t="s">
         <v>737</v>
-      </c>
-      <c r="D279" s="26" t="s">
-        <v>742</v>
       </c>
       <c r="E279" s="80" t="s">
         <v>157</v>
@@ -19670,10 +19670,10 @@
         <v>60</v>
       </c>
       <c r="C280" s="32" t="s">
+        <v>733</v>
+      </c>
+      <c r="D280" s="26" t="s">
         <v>738</v>
-      </c>
-      <c r="D280" s="26" t="s">
-        <v>743</v>
       </c>
       <c r="E280" s="80" t="s">
         <v>157</v>
@@ -19698,7 +19698,7 @@
         <v>61</v>
       </c>
       <c r="C281" s="32" t="s">
-        <v>729</v>
+        <v>724</v>
       </c>
       <c r="D281" s="26" t="s">
         <v>618</v>
@@ -19726,7 +19726,7 @@
         <v>62</v>
       </c>
       <c r="C282" s="32" t="s">
-        <v>730</v>
+        <v>725</v>
       </c>
       <c r="D282" s="26" t="s">
         <v>409</v>
@@ -19752,7 +19752,7 @@
         <v>63</v>
       </c>
       <c r="C283" s="32" t="s">
-        <v>731</v>
+        <v>726</v>
       </c>
       <c r="D283" s="26" t="s">
         <v>410</v>

</xml_diff>